<commit_message>
Updated on 2022-05-17 11:24:50
</commit_message>
<xml_diff>
--- a/data/result_headers.xlsx
+++ b/data/result_headers.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Azim\2022\lju-result\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AF6B2D-9D38-4F2F-B4F3-0940113B4EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133F048B-345F-4440-A4DF-F122C725111D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{872E6430-57B9-462A-A727-3B07EE4A426E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{872E6430-57B9-462A-A727-3B07EE4A426E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="349">
   <si>
     <t>Institution=str(df["Institution"][tindex]),</t>
   </si>
@@ -1045,6 +1046,42 @@
   </si>
   <si>
     <t>Mark_10_OA</t>
+  </si>
+  <si>
+    <t>Date1</t>
+  </si>
+  <si>
+    <t>Date2</t>
+  </si>
+  <si>
+    <t>Date3</t>
+  </si>
+  <si>
+    <t>Date4</t>
+  </si>
+  <si>
+    <t>Date5</t>
+  </si>
+  <si>
+    <t>Date6</t>
+  </si>
+  <si>
+    <t>Time1</t>
+  </si>
+  <si>
+    <t>Time2</t>
+  </si>
+  <si>
+    <t>Time3</t>
+  </si>
+  <si>
+    <t>Time4</t>
+  </si>
+  <si>
+    <t>Time5</t>
+  </si>
+  <si>
+    <t>Time6</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95D5A6A-C9B4-4A65-B975-D19B1B4FE22E}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3582,4 +3619,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCDC0A3-A8A9-4F14-8FFE-E9FEF575207C}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" t="str">
+        <f>A1&amp;"=str(df[*"&amp;A1&amp;"*][tindex]),"</f>
+        <v>InstituteCode=str(df[*InstituteCode*][tindex]),</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B27" si="0">A2&amp;"=str(df[*"&amp;A2&amp;"*][tindex]),"</f>
+        <v>ExamName=str(df[*ExamName*][tindex]),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>ExamMonthYear=str(df[*ExamMonthYear*][tindex]),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Semester=str(df[*Semester*][tindex]),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>SeatNo=str(df[*SeatNo*][tindex]),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>EnrolmentNo=str(df[*EnrolmentNo*][tindex]),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>StudentName=str(df[*StudentName*][tindex]),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>ProgramCode=str(df[*ProgramCode*][tindex]),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>BranchCode=str(df[*BranchCode*][tindex]),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Sub1=str(df[*Sub1*][tindex]),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Sub2=str(df[*Sub2*][tindex]),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sub3=str(df[*Sub3*][tindex]),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Sub4=str(df[*Sub4*][tindex]),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Sub5=str(df[*Sub5*][tindex]),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Sub6=str(df[*Sub6*][tindex]),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>337</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Date1=str(df[*Date1*][tindex]),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>338</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Date2=str(df[*Date2*][tindex]),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Date3=str(df[*Date3*][tindex]),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Date4=str(df[*Date4*][tindex]),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>341</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Date5=str(df[*Date5*][tindex]),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>342</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Date6=str(df[*Date6*][tindex]),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>343</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Time1=str(df[*Time1*][tindex]),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>344</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Time2=str(df[*Time2*][tindex]),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Time3=str(df[*Time3*][tindex]),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>346</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Time4=str(df[*Time4*][tindex]),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>347</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>Time5=str(df[*Time5*][tindex]),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>348</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>Time6=str(df[*Time6*][tindex]),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>